<commit_message>
duzi - new slide in the pptx file and new xlsx file
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V3.xlsx
+++ b/Test Enviroment Plan V3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduardo_spirito\Documents\Syngenta ASM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T966104\Documents\repos\docs\syngenta-appmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Enviroment Detail" sheetId="1" r:id="rId1"/>
     <sheet name="TimeLine" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -740,6 +740,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,9 +776,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,27 +786,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1081,7 @@
     <col min="2" max="2" width="8.85546875" style="2"/>
     <col min="3" max="3" width="42.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="42.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1893,22 +1893,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="54"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="11" t="s">
         <v>62</v>
       </c>
@@ -1932,16 +1932,16 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="54"/>
+      <c r="F2" s="44"/>
       <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
@@ -1965,23 +1965,23 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="52" t="s">
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1993,8 +1993,8 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="1"/>
@@ -2014,8 +2014,8 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="43"/>
-      <c r="E5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
       <c r="H5" s="1"/>
@@ -2029,20 +2029,20 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="52" t="s">
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2054,9 +2054,9 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="12"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2075,9 +2075,9 @@
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="12"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2096,9 +2096,9 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="12"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2117,9 +2117,9 @@
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="12"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2138,9 +2138,9 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="12"/>
       <c r="H11" s="1"/>
       <c r="I11" s="14"/>
@@ -2159,9 +2159,9 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
       <c r="G12" s="12"/>
       <c r="H12" s="14"/>
       <c r="I12" s="1"/>
@@ -2180,9 +2180,9 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="12"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2201,9 +2201,9 @@
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="12"/>
       <c r="H14" s="1"/>
       <c r="I14" s="14"/>
@@ -2222,9 +2222,9 @@
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
       <c r="G15" s="12"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2243,9 +2243,9 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="12"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2264,9 +2264,9 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
       <c r="G17" s="12"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2285,9 +2285,9 @@
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2306,9 +2306,9 @@
       <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
       <c r="G19" s="18"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -2327,9 +2327,9 @@
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
       <c r="G20" s="12"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2340,11 +2340,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D7:F7"/>
@@ -2359,13 +2361,11 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>